<commit_message>
Changes to several parts, still in doubt about the dual pricing problems
</commit_message>
<xml_diff>
--- a/Example_Data_PMF.xlsx
+++ b/Example_Data_PMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49fd97070908fc11/6. TU Delft/AE4423 - Airline Planning and Optimization/AE4426/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{E5F21EBE-6982-E345-BD8E-7D2E9A919D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{718B6DF4-5A40-924C-B7FC-F25ABA3AC97F}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{E5F21EBE-6982-E345-BD8E-7D2E9A919D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F45FF01B-3D51-5D43-B8C4-925E54D5BD89}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -702,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -1269,7 +1269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>